<commit_message>
new outputs from multiprocessing execution
</commit_message>
<xml_diff>
--- a/results/ner_alternatives_statistics.xlsx
+++ b/results/ner_alternatives_statistics.xlsx
@@ -508,47 +508,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>gpt_4o_mini</t>
+          <t>fine_tuned_gpt_4o_mini</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5153654867664156</v>
+        <v>0.6507966344243519</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6707104527417028</v>
+        <v>0.6455199314574315</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5682982187558271</v>
+        <v>0.6364691594862174</v>
       </c>
       <c r="E2" t="n">
-        <v>70.96273291925466</v>
+        <v>65.21739130434783</v>
       </c>
       <c r="F2" t="n">
-        <v>41.92546583850932</v>
+        <v>56.52173913043478</v>
       </c>
       <c r="G2" t="n">
-        <v>10.94091903719912</v>
+        <v>16.90476190476191</v>
       </c>
       <c r="H2" t="n">
-        <v>18.16192560175055</v>
+        <v>28.09523809523809</v>
       </c>
       <c r="I2" t="n">
-        <v>22.5382932166302</v>
+        <v>36.19047619047619</v>
       </c>
       <c r="J2" t="n">
-        <v>28.44638949671772</v>
+        <v>45.95238095238095</v>
       </c>
       <c r="K2" t="n">
-        <v>4.814004376367615</v>
+        <v>15.47619047619048</v>
       </c>
       <c r="L2" t="n">
-        <v>15.53610503282276</v>
+        <v>27.61904761904762</v>
       </c>
       <c r="M2" t="n">
-        <v>21.44420131291028</v>
+        <v>35.71428571428572</v>
       </c>
       <c r="N2" t="n">
-        <v>28.00875273522976</v>
+        <v>45.95238095238095</v>
       </c>
     </row>
     <row r="3">
@@ -558,135 +558,135 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6805618375253631</v>
+        <v>0.6843809432830815</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6977158113876865</v>
+        <v>0.6985712782587784</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6816539326841841</v>
+        <v>0.6808901394872756</v>
       </c>
       <c r="E3" t="n">
-        <v>73.75776397515527</v>
+        <v>72.67080745341616</v>
       </c>
       <c r="F3" t="n">
-        <v>66.77018633540372</v>
+        <v>64.13043478260869</v>
       </c>
       <c r="G3" t="n">
-        <v>20</v>
+        <v>19.87179487179487</v>
       </c>
       <c r="H3" t="n">
-        <v>38.31578947368421</v>
+        <v>35.04273504273504</v>
       </c>
       <c r="I3" t="n">
-        <v>49.47368421052632</v>
+        <v>50.85470085470085</v>
       </c>
       <c r="J3" t="n">
-        <v>61.68421052631579</v>
+        <v>62.39316239316239</v>
       </c>
       <c r="K3" t="n">
-        <v>17.26315789473684</v>
+        <v>17.73504273504274</v>
       </c>
       <c r="L3" t="n">
-        <v>37.68421052631579</v>
+        <v>34.4017094017094</v>
       </c>
       <c r="M3" t="n">
-        <v>49.89473684210527</v>
+        <v>50.85470085470085</v>
       </c>
       <c r="N3" t="n">
-        <v>61.47368421052632</v>
+        <v>62.17948717948718</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>fine_tuned_gpt_4o_v2</t>
+          <t>fine_tuned_gpt_4o_mini_v2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8336817696192697</v>
+        <v>0.8562024897414151</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8210843554593555</v>
+        <v>0.8599851537351538</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8191987032467912</v>
+        <v>0.8538762209899445</v>
       </c>
       <c r="E4" t="n">
-        <v>82.29813664596274</v>
+        <v>84.93788819875776</v>
       </c>
       <c r="F4" t="n">
-        <v>75.93167701863354</v>
+        <v>75.77639751552795</v>
       </c>
       <c r="G4" t="n">
-        <v>25.09433962264151</v>
+        <v>21.57221206581353</v>
       </c>
       <c r="H4" t="n">
-        <v>48.30188679245283</v>
+        <v>34.55210237659963</v>
       </c>
       <c r="I4" t="n">
-        <v>58.30188679245283</v>
+        <v>49.90859232175503</v>
       </c>
       <c r="J4" t="n">
-        <v>74.52830188679245</v>
+        <v>61.42595978062158</v>
       </c>
       <c r="K4" t="n">
-        <v>24.33962264150943</v>
+        <v>20.84095063985375</v>
       </c>
       <c r="L4" t="n">
-        <v>48.30188679245283</v>
+        <v>34.36928702010969</v>
       </c>
       <c r="M4" t="n">
-        <v>58.30188679245283</v>
+        <v>49.72577696526508</v>
       </c>
       <c r="N4" t="n">
-        <v>74.52830188679245</v>
+        <v>61.24314442413162</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>fine_tuned_gpt_4o_mini</t>
+          <t>fine_tuned_gpt_4o_v2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6190007267539678</v>
+        <v>0.8102967337547931</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6354791186822437</v>
+        <v>0.8163485675204426</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6118222939680261</v>
+        <v>0.8040474712754717</v>
       </c>
       <c r="E5" t="n">
-        <v>65.83850931677019</v>
+        <v>81.67701863354037</v>
       </c>
       <c r="F5" t="n">
-        <v>57.91925465838509</v>
+        <v>75.62111801242236</v>
       </c>
       <c r="G5" t="n">
-        <v>14.15094339622642</v>
+        <v>30.03802281368822</v>
       </c>
       <c r="H5" t="n">
-        <v>28.06603773584906</v>
+        <v>45.81749049429658</v>
       </c>
       <c r="I5" t="n">
-        <v>36.08490566037736</v>
+        <v>60.45627376425855</v>
       </c>
       <c r="J5" t="n">
-        <v>42.9245283018868</v>
+        <v>69.01140684410646</v>
       </c>
       <c r="K5" t="n">
-        <v>12.5</v>
+        <v>30.03802281368822</v>
       </c>
       <c r="L5" t="n">
-        <v>27.59433962264151</v>
+        <v>45.81749049429658</v>
       </c>
       <c r="M5" t="n">
-        <v>35.84905660377358</v>
+        <v>60.26615969581749</v>
       </c>
       <c r="N5" t="n">
-        <v>42.9245283018868</v>
+        <v>69.01140684410646</v>
       </c>
     </row>
     <row r="6">
@@ -696,181 +696,181 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6743224368224369</v>
+        <v>0.7619155036301417</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7233658702408702</v>
+        <v>0.8016875919219669</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6871873217942887</v>
+        <v>0.7684494353043774</v>
       </c>
       <c r="E6" t="n">
-        <v>72.98136645962732</v>
+        <v>74.04921700223713</v>
       </c>
       <c r="F6" t="n">
-        <v>56.83229813664597</v>
+        <v>45.63758389261745</v>
       </c>
       <c r="G6" t="n">
-        <v>21.91489361702128</v>
+        <v>25.98187311178248</v>
       </c>
       <c r="H6" t="n">
-        <v>32.76595744680851</v>
+        <v>39.57703927492447</v>
       </c>
       <c r="I6" t="n">
-        <v>40.63829787234042</v>
+        <v>51.05740181268882</v>
       </c>
       <c r="J6" t="n">
-        <v>50.42553191489362</v>
+        <v>59.21450151057401</v>
       </c>
       <c r="K6" t="n">
-        <v>18.72340425531915</v>
+        <v>21.45015105740181</v>
       </c>
       <c r="L6" t="n">
-        <v>32.3404255319149</v>
+        <v>37.76435045317221</v>
       </c>
       <c r="M6" t="n">
-        <v>40.42553191489361</v>
+        <v>51.3595166163142</v>
       </c>
       <c r="N6" t="n">
-        <v>49.78723404255319</v>
+        <v>59.21450151057401</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sonnet_35</t>
+          <t>gliner</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6375702348717355</v>
+        <v>0.6532512626262627</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7701589932058682</v>
+        <v>0.4476419992044993</v>
       </c>
       <c r="D7" t="n">
-        <v>0.681905990462128</v>
+        <v>0.506185989190214</v>
       </c>
       <c r="E7" t="n">
-        <v>77.63975155279503</v>
+        <v>51.24223602484472</v>
       </c>
       <c r="F7" t="n">
-        <v>67.70186335403726</v>
+        <v>20.3416149068323</v>
       </c>
       <c r="G7" t="n">
-        <v>18.6</v>
+        <v>98.7878787878788</v>
       </c>
       <c r="H7" t="n">
-        <v>39.8</v>
+        <v>98.7878787878788</v>
       </c>
       <c r="I7" t="n">
-        <v>55.8</v>
+        <v>98.7878787878788</v>
       </c>
       <c r="J7" t="n">
-        <v>65.8</v>
+        <v>99.09090909090909</v>
       </c>
       <c r="K7" t="n">
-        <v>15.6</v>
+        <v>98.7878787878788</v>
       </c>
       <c r="L7" t="n">
-        <v>39.6</v>
+        <v>98.7878787878788</v>
       </c>
       <c r="M7" t="n">
-        <v>55.60000000000001</v>
+        <v>98.7878787878788</v>
       </c>
       <c r="N7" t="n">
-        <v>65.8</v>
+        <v>99.09090909090909</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>gliner</t>
+          <t>gpt_4o_mini</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6532512626262627</v>
+        <v>0.5237153074477313</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4476419992044993</v>
+        <v>0.6889567174723424</v>
       </c>
       <c r="D8" t="n">
-        <v>0.506185989190214</v>
+        <v>0.5736679606668337</v>
       </c>
       <c r="E8" t="n">
-        <v>51.24223602484472</v>
+        <v>68.63354037267081</v>
       </c>
       <c r="F8" t="n">
-        <v>20.3416149068323</v>
+        <v>39.59627329192546</v>
       </c>
       <c r="G8" t="n">
-        <v>98.7878787878788</v>
+        <v>11.08597285067873</v>
       </c>
       <c r="H8" t="n">
-        <v>98.7878787878788</v>
+        <v>18.09954751131222</v>
       </c>
       <c r="I8" t="n">
-        <v>98.7878787878788</v>
+        <v>22.85067873303167</v>
       </c>
       <c r="J8" t="n">
-        <v>99.09090909090909</v>
+        <v>28.28054298642534</v>
       </c>
       <c r="K8" t="n">
-        <v>98.7878787878788</v>
+        <v>6.108597285067873</v>
       </c>
       <c r="L8" t="n">
-        <v>98.7878787878788</v>
+        <v>16.7420814479638</v>
       </c>
       <c r="M8" t="n">
-        <v>98.7878787878788</v>
+        <v>23.30316742081448</v>
       </c>
       <c r="N8" t="n">
-        <v>99.09090909090909</v>
+        <v>27.14932126696833</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>fine_tuned_gpt_4o_mini_v2</t>
+          <t>sonnet_35</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.866629895329344</v>
+        <v>0.6317338963025781</v>
       </c>
       <c r="C9" t="n">
-        <v>0.864564500892626</v>
+        <v>0.7606979392135642</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8585306294818564</v>
+        <v>0.6731942184922062</v>
       </c>
       <c r="E9" t="n">
-        <v>84.78260869565217</v>
+        <v>76.86335403726709</v>
       </c>
       <c r="F9" t="n">
-        <v>76.24223602484473</v>
+        <v>67.2360248447205</v>
       </c>
       <c r="G9" t="n">
-        <v>20.32967032967033</v>
+        <v>23.83838383838384</v>
       </c>
       <c r="H9" t="n">
-        <v>37.17948717948718</v>
+        <v>38.98989898989899</v>
       </c>
       <c r="I9" t="n">
-        <v>53.11355311355312</v>
+        <v>51.71717171717172</v>
       </c>
       <c r="J9" t="n">
-        <v>63.36996336996337</v>
+        <v>62.22222222222222</v>
       </c>
       <c r="K9" t="n">
-        <v>19.5970695970696</v>
+        <v>20</v>
       </c>
       <c r="L9" t="n">
-        <v>37.17948717948718</v>
+        <v>38.98989898989899</v>
       </c>
       <c r="M9" t="n">
-        <v>53.11355311355312</v>
+        <v>51.71717171717172</v>
       </c>
       <c r="N9" t="n">
-        <v>63.36996336996337</v>
+        <v>62.02020202020202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>